<commit_message>
created filter 50% of the filter options
</commit_message>
<xml_diff>
--- a/server/src/main/resources/dataExcel/Students.xlsx
+++ b/server/src/main/resources/dataExcel/Students.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Dev\SCS_ANP\server\src\main\resources\dataExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Dev\PERA ALUMNI\SCS_ANP\server\src\main\resources\dataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636FAA52-B100-4EB0-B2CE-DF3E8B3765FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424BAB66-1024-46AE-BA0B-9A65D0317796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data17" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet 01" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="225">
   <si>
     <t>reg_No</t>
   </si>
@@ -680,6 +680,21 @@
   </si>
   <si>
     <t>7776665555v</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>STAT</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>isOpentoWork</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,9 +1557,11 @@
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="22.42578125" customWidth="1"/>
     <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1587,8 +1604,14 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>220</v>
+      </c>
+      <c r="P1" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>17001</v>
       </c>
@@ -1605,13 +1628,13 @@
         <v>17</v>
       </c>
       <c r="F2">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -1631,10 +1654,16 @@
       <c r="N2" t="s">
         <v>23</v>
       </c>
+      <c r="O2" t="s">
+        <v>221</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>17002</v>
+        <v>18002</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -1649,7 +1678,7 @@
         <v>27</v>
       </c>
       <c r="F3">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
@@ -1675,10 +1704,16 @@
       <c r="N3" t="s">
         <v>32</v>
       </c>
+      <c r="O3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>17003</v>
+        <v>18003</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -1693,13 +1728,13 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="G4" t="s">
         <v>36</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>37</v>
@@ -1719,8 +1754,14 @@
       <c r="N4" t="s">
         <v>40</v>
       </c>
+      <c r="O4" t="s">
+        <v>221</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17004</v>
       </c>
@@ -1737,13 +1778,13 @@
         <v>27</v>
       </c>
       <c r="F5">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G5" t="s">
         <v>44</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="s">
         <v>45</v>
@@ -1763,8 +1804,14 @@
       <c r="N5" t="s">
         <v>48</v>
       </c>
+      <c r="O5" t="s">
+        <v>221</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>17005</v>
       </c>
@@ -1781,7 +1828,7 @@
         <v>17</v>
       </c>
       <c r="F6">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
@@ -1807,8 +1854,14 @@
       <c r="N6" t="s">
         <v>56</v>
       </c>
+      <c r="O6" t="s">
+        <v>221</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>17006</v>
       </c>
@@ -1825,13 +1878,13 @@
         <v>27</v>
       </c>
       <c r="F7">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="G7" t="s">
         <v>60</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>61</v>
@@ -1851,8 +1904,14 @@
       <c r="N7" t="s">
         <v>64</v>
       </c>
+      <c r="O7" t="s">
+        <v>221</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>17317</v>
       </c>
@@ -1869,13 +1928,13 @@
         <v>17</v>
       </c>
       <c r="F8">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G8" t="s">
         <v>68</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="s">
         <v>69</v>
@@ -1895,8 +1954,14 @@
       <c r="N8" t="s">
         <v>72</v>
       </c>
+      <c r="O8" t="s">
+        <v>223</v>
+      </c>
+      <c r="P8" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17318</v>
       </c>
@@ -1913,7 +1978,7 @@
         <v>27</v>
       </c>
       <c r="F9">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="G9" t="s">
         <v>76</v>
@@ -1939,8 +2004,14 @@
       <c r="N9" t="s">
         <v>80</v>
       </c>
+      <c r="O9" t="s">
+        <v>223</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17319</v>
       </c>
@@ -1957,13 +2028,13 @@
         <v>17</v>
       </c>
       <c r="F10">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="G10" t="s">
         <v>84</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="s">
         <v>85</v>
@@ -1983,10 +2054,16 @@
       <c r="N10" t="s">
         <v>88</v>
       </c>
+      <c r="O10" t="s">
+        <v>223</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>17320</v>
+        <v>18320</v>
       </c>
       <c r="B11" t="s">
         <v>89</v>
@@ -2001,13 +2078,13 @@
         <v>27</v>
       </c>
       <c r="F11">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G11" t="s">
         <v>92</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
         <v>93</v>
@@ -2027,10 +2104,16 @@
       <c r="N11" t="s">
         <v>96</v>
       </c>
+      <c r="O11" t="s">
+        <v>223</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>17411</v>
+        <v>18411</v>
       </c>
       <c r="B12" t="s">
         <v>97</v>
@@ -2045,7 +2128,7 @@
         <v>17</v>
       </c>
       <c r="F12">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="G12" t="s">
         <v>100</v>
@@ -2071,10 +2154,16 @@
       <c r="N12" t="s">
         <v>104</v>
       </c>
+      <c r="O12" t="s">
+        <v>223</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>17412</v>
+        <v>18412</v>
       </c>
       <c r="B13" t="s">
         <v>105</v>
@@ -2089,13 +2178,13 @@
         <v>27</v>
       </c>
       <c r="F13">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="G13" t="s">
         <v>108</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>109</v>
@@ -2115,8 +2204,14 @@
       <c r="N13" t="s">
         <v>112</v>
       </c>
+      <c r="O13" t="s">
+        <v>223</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>17413</v>
       </c>
@@ -2133,13 +2228,13 @@
         <v>17</v>
       </c>
       <c r="F14">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G14" t="s">
         <v>116</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>117</v>
@@ -2159,8 +2254,14 @@
       <c r="N14" t="s">
         <v>120</v>
       </c>
+      <c r="O14" t="s">
+        <v>223</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>17414</v>
       </c>
@@ -2177,7 +2278,7 @@
         <v>27</v>
       </c>
       <c r="F15">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="G15" t="s">
         <v>124</v>
@@ -2203,8 +2304,14 @@
       <c r="N15" t="s">
         <v>128</v>
       </c>
+      <c r="O15" t="s">
+        <v>223</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17415</v>
       </c>
@@ -2221,13 +2328,13 @@
         <v>17</v>
       </c>
       <c r="F16">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="G16" t="s">
         <v>132</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="s">
         <v>133</v>
@@ -2247,8 +2354,14 @@
       <c r="N16" t="s">
         <v>80</v>
       </c>
+      <c r="O16" t="s">
+        <v>221</v>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17516</v>
       </c>
@@ -2265,13 +2378,13 @@
         <v>27</v>
       </c>
       <c r="F17">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G17" t="s">
         <v>92</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="s">
         <v>135</v>
@@ -2291,8 +2404,14 @@
       <c r="N17" t="s">
         <v>96</v>
       </c>
+      <c r="O17" t="s">
+        <v>223</v>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17517</v>
       </c>
@@ -2309,7 +2428,7 @@
         <v>17</v>
       </c>
       <c r="F18">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="G18" t="s">
         <v>139</v>
@@ -2335,10 +2454,16 @@
       <c r="N18" t="s">
         <v>143</v>
       </c>
+      <c r="O18" t="s">
+        <v>222</v>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17518</v>
+        <v>18518</v>
       </c>
       <c r="B19" t="s">
         <v>144</v>
@@ -2353,13 +2478,13 @@
         <v>27</v>
       </c>
       <c r="F19">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="G19" t="s">
         <v>147</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>45</v>
@@ -2379,10 +2504,16 @@
       <c r="N19" t="s">
         <v>150</v>
       </c>
+      <c r="O19" t="s">
+        <v>222</v>
+      </c>
+      <c r="P19" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>17519</v>
+        <v>18519</v>
       </c>
       <c r="B20" t="s">
         <v>151</v>
@@ -2397,13 +2528,13 @@
         <v>17</v>
       </c>
       <c r="F20">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G20" t="s">
         <v>154</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
         <v>155</v>
@@ -2423,10 +2554,16 @@
       <c r="N20" t="s">
         <v>158</v>
       </c>
+      <c r="O20" t="s">
+        <v>222</v>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>17520</v>
+        <v>18520</v>
       </c>
       <c r="B21" t="s">
         <v>159</v>
@@ -2441,7 +2578,7 @@
         <v>27</v>
       </c>
       <c r="F21">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="G21" t="s">
         <v>162</v>
@@ -2467,8 +2604,14 @@
       <c r="N21" t="s">
         <v>165</v>
       </c>
+      <c r="O21" t="s">
+        <v>222</v>
+      </c>
+      <c r="P21" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17821</v>
       </c>
@@ -2485,13 +2628,13 @@
         <v>17</v>
       </c>
       <c r="F22">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="G22" t="s">
         <v>169</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="s">
         <v>93</v>
@@ -2511,8 +2654,14 @@
       <c r="N22" t="s">
         <v>172</v>
       </c>
+      <c r="O22" t="s">
+        <v>222</v>
+      </c>
+      <c r="P22" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17822</v>
       </c>
@@ -2529,13 +2678,13 @@
         <v>27</v>
       </c>
       <c r="F23">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G23" t="s">
         <v>176</v>
       </c>
       <c r="H23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="s">
         <v>101</v>
@@ -2555,8 +2704,14 @@
       <c r="N23" t="s">
         <v>179</v>
       </c>
+      <c r="O23" t="s">
+        <v>222</v>
+      </c>
+      <c r="P23" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17823</v>
       </c>
@@ -2573,7 +2728,7 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="G24" t="s">
         <v>183</v>
@@ -2599,8 +2754,14 @@
       <c r="N24" t="s">
         <v>187</v>
       </c>
+      <c r="O24" t="s">
+        <v>222</v>
+      </c>
+      <c r="P24" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17824</v>
       </c>
@@ -2617,13 +2778,13 @@
         <v>27</v>
       </c>
       <c r="F25">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="G25" t="s">
         <v>191</v>
       </c>
       <c r="H25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
         <v>155</v>
@@ -2643,8 +2804,14 @@
       <c r="N25" t="s">
         <v>194</v>
       </c>
+      <c r="O25" t="s">
+        <v>222</v>
+      </c>
+      <c r="P25" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17825</v>
       </c>
@@ -2661,13 +2828,13 @@
         <v>17</v>
       </c>
       <c r="F26">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G26" t="s">
         <v>197</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="s">
         <v>140</v>
@@ -2686,6 +2853,12 @@
       </c>
       <c r="N26" t="s">
         <v>200</v>
+      </c>
+      <c r="O26" t="s">
+        <v>222</v>
+      </c>
+      <c r="P26" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>